<commit_message>
added openpyxl and excel
</commit_message>
<xml_diff>
--- a/data/Auswertungen.xlsx
+++ b/data/Auswertungen.xlsx
@@ -11,7 +11,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+  <si>
+    <t>Jahr</t>
+  </si>
   <si>
     <t>Datum</t>
   </si>
@@ -168,7 +171,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="dd.mm.yyyy"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -180,13 +183,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,6 +210,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="12"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -226,6 +240,21 @@
       </top>
       <bottom style="thin">
         <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -267,7 +296,7 @@
         <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="10"/>
@@ -304,68 +333,62 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="3" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="3" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -389,6 +412,7 @@
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffffffff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -405,10 +429,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -585,11 +609,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -598,7 +625,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -612,19 +639,19 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -863,12 +890,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1149,7 +1176,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1417,17 +1444,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AN22"/>
+  <dimension ref="A1:AO22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B2" xSplit="1" ySplit="1" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="1" customWidth="1"/>
-    <col min="7" max="40" width="18.8828" style="1" customWidth="1"/>
-    <col min="41" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
+    <col min="8" max="41" width="18.8516" style="1" customWidth="1"/>
+    <col min="42" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20.25" customHeight="1">
@@ -1551,1508 +1576,1548 @@
       <c r="AN1" t="s" s="2">
         <v>39</v>
       </c>
+      <c r="AO1" t="s" s="2">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" ht="20.25" customHeight="1">
       <c r="A2" s="3">
+        <v>2023</v>
+      </c>
+      <c r="B2" s="4">
         <v>45158</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>40</v>
       </c>
       <c r="C2" t="s" s="5">
         <v>41</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" t="s" s="6">
+        <v>42</v>
+      </c>
+      <c r="E2" s="7">
         <v>23</v>
       </c>
-      <c r="E2" s="6">
+      <c r="F2" s="7">
         <v>6.6</v>
       </c>
-      <c r="F2" s="6">
+      <c r="G2" s="7">
         <v>4.33</v>
       </c>
-      <c r="G2" s="6">
-        <v>16</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="H2" s="7">
+        <v>16</v>
+      </c>
+      <c r="I2" s="7">
         <v>10.93</v>
       </c>
-      <c r="I2" s="6">
+      <c r="J2" s="7">
         <v>4.41</v>
       </c>
-      <c r="J2" s="6">
-        <v>16</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="K2" s="7">
+        <v>16</v>
+      </c>
+      <c r="L2" s="7">
         <v>15.34</v>
       </c>
-      <c r="L2" s="6">
+      <c r="M2" s="7">
         <v>4.5</v>
       </c>
-      <c r="M2" s="6">
-        <v>16</v>
-      </c>
-      <c r="N2" s="6">
+      <c r="N2" s="7">
+        <v>16</v>
+      </c>
+      <c r="O2" s="7">
         <v>19.84</v>
       </c>
-      <c r="O2" s="6">
+      <c r="P2" s="7">
         <v>4.65</v>
       </c>
-      <c r="P2" s="6">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="6">
+      <c r="Q2" s="7">
+        <v>16</v>
+      </c>
+      <c r="R2" s="7">
         <v>24.49</v>
       </c>
-      <c r="R2" s="6">
+      <c r="S2" s="7">
         <v>26.36</v>
       </c>
-      <c r="S2" s="6">
+      <c r="T2" s="7">
         <v>4.67</v>
       </c>
-      <c r="T2" s="6">
-        <v>16</v>
-      </c>
-      <c r="U2" s="6">
+      <c r="U2" s="7">
+        <v>16</v>
+      </c>
+      <c r="V2" s="7">
         <v>29.16</v>
       </c>
-      <c r="V2" s="6">
+      <c r="W2" s="7">
         <v>4.86</v>
       </c>
-      <c r="W2" s="6">
-        <v>16</v>
-      </c>
-      <c r="X2" s="6">
+      <c r="X2" s="7">
+        <v>16</v>
+      </c>
+      <c r="Y2" s="7">
         <v>34.02</v>
       </c>
-      <c r="Y2" s="6">
+      <c r="Z2" s="7">
         <v>5.12</v>
       </c>
-      <c r="Z2" s="6">
+      <c r="AA2" s="7">
         <v>17</v>
       </c>
-      <c r="AA2" s="6">
+      <c r="AB2" s="7">
         <v>39.14</v>
       </c>
-      <c r="AB2" s="6">
+      <c r="AC2" s="7">
         <v>5.25</v>
       </c>
-      <c r="AC2" s="6">
+      <c r="AD2" s="7">
         <v>17</v>
       </c>
-      <c r="AD2" s="6">
+      <c r="AE2" s="7">
         <v>44.39</v>
       </c>
-      <c r="AE2" s="6">
+      <c r="AF2" s="7">
         <v>5.29</v>
       </c>
-      <c r="AF2" s="6">
+      <c r="AG2" s="7">
         <v>17</v>
       </c>
-      <c r="AG2" s="6">
+      <c r="AH2" s="7">
         <v>49.68</v>
       </c>
-      <c r="AH2" s="6">
+      <c r="AI2" s="7">
         <v>5.95</v>
       </c>
-      <c r="AI2" s="6">
+      <c r="AJ2" s="7">
         <v>55.63</v>
       </c>
-      <c r="AJ2" s="6">
+      <c r="AK2" s="7">
         <v>26.36</v>
       </c>
-      <c r="AK2" s="6">
+      <c r="AL2" s="7">
         <v>29.27</v>
       </c>
-      <c r="AL2" s="6">
+      <c r="AM2" s="7">
         <v>2.91</v>
       </c>
-      <c r="AM2" s="6">
+      <c r="AN2" s="7">
         <v>1</v>
       </c>
-      <c r="AN2" s="6">
+      <c r="AO2" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="3" ht="20.05" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B3" s="9">
         <v>45431</v>
       </c>
-      <c r="B3" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="C3" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s" s="11">
+        <v>43</v>
+      </c>
+      <c r="E3" s="12">
         <v>23</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="10">
+      <c r="F3" s="13"/>
+      <c r="G3" s="12">
         <v>0</v>
       </c>
-      <c r="G3" s="10">
+      <c r="H3" s="12">
         <v>15</v>
       </c>
-      <c r="H3" s="11"/>
-      <c r="I3" s="10">
+      <c r="I3" s="13"/>
+      <c r="J3" s="12">
         <v>0</v>
       </c>
-      <c r="J3" s="10">
+      <c r="K3" s="12">
         <v>15</v>
       </c>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10">
+      <c r="L3" s="13"/>
+      <c r="M3" s="12">
         <v>0</v>
       </c>
-      <c r="M3" s="10">
-        <v>16</v>
-      </c>
-      <c r="N3" s="11"/>
-      <c r="O3" s="10">
+      <c r="N3" s="12">
+        <v>16</v>
+      </c>
+      <c r="O3" s="13"/>
+      <c r="P3" s="12">
         <v>0</v>
       </c>
-      <c r="P3" s="10">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="10">
+      <c r="Q3" s="12">
+        <v>16</v>
+      </c>
+      <c r="R3" s="13"/>
+      <c r="S3" s="12">
         <v>0</v>
       </c>
-      <c r="S3" s="10">
+      <c r="T3" s="12">
         <v>0</v>
       </c>
-      <c r="T3" s="10">
-        <v>16</v>
-      </c>
-      <c r="U3" s="11"/>
-      <c r="V3" s="10">
+      <c r="U3" s="12">
+        <v>16</v>
+      </c>
+      <c r="V3" s="13"/>
+      <c r="W3" s="12">
         <v>0</v>
       </c>
-      <c r="W3" s="10">
-        <v>16</v>
-      </c>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="10">
+      <c r="X3" s="12">
+        <v>16</v>
+      </c>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="12">
         <v>0</v>
       </c>
-      <c r="Z3" s="10">
+      <c r="AA3" s="12">
         <v>17</v>
       </c>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="10">
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="12">
         <v>0</v>
       </c>
-      <c r="AC3" s="10">
+      <c r="AD3" s="12">
         <v>17</v>
       </c>
-      <c r="AD3" s="11"/>
-      <c r="AE3" s="10">
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="12">
         <v>0</v>
       </c>
-      <c r="AF3" s="10">
+      <c r="AG3" s="12">
         <v>19</v>
       </c>
-      <c r="AG3" s="11"/>
-      <c r="AH3" s="10">
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="12">
         <v>0</v>
       </c>
-      <c r="AI3" s="10">
+      <c r="AJ3" s="12">
         <v>58.22</v>
       </c>
-      <c r="AJ3" s="10">
+      <c r="AK3" s="12">
         <v>0</v>
       </c>
-      <c r="AK3" s="10">
+      <c r="AL3" s="12">
         <v>0</v>
       </c>
-      <c r="AL3" s="10">
+      <c r="AM3" s="12">
         <v>0</v>
       </c>
-      <c r="AM3" s="10">
+      <c r="AN3" s="12">
         <v>7</v>
       </c>
-      <c r="AN3" s="10">
+      <c r="AO3" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="7">
+      <c r="A4" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B4" s="9">
         <v>45432</v>
       </c>
-      <c r="B4" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="C4" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="C4" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s" s="11">
+        <v>44</v>
+      </c>
+      <c r="E4" s="12">
         <v>23</v>
       </c>
-      <c r="E4" s="10">
+      <c r="F4" s="12">
         <v>6.72</v>
       </c>
-      <c r="F4" s="10">
+      <c r="G4" s="12">
         <v>4.27</v>
       </c>
-      <c r="G4" s="10">
+      <c r="H4" s="12">
         <v>15</v>
       </c>
-      <c r="H4" s="10">
+      <c r="I4" s="12">
         <v>10.99</v>
       </c>
-      <c r="I4" s="10">
+      <c r="J4" s="12">
         <v>4.39</v>
       </c>
-      <c r="J4" s="10">
+      <c r="K4" s="12">
         <v>15</v>
       </c>
-      <c r="K4" s="10">
+      <c r="L4" s="12">
         <v>15.38</v>
       </c>
-      <c r="L4" s="10">
+      <c r="M4" s="12">
         <v>4.58</v>
       </c>
-      <c r="M4" s="10">
-        <v>16</v>
-      </c>
-      <c r="N4" s="10">
+      <c r="N4" s="12">
+        <v>16</v>
+      </c>
+      <c r="O4" s="12">
         <v>19.96</v>
       </c>
-      <c r="O4" s="10">
+      <c r="P4" s="12">
         <v>4.71</v>
       </c>
-      <c r="P4" s="10">
-        <v>16</v>
-      </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="12">
+        <v>16</v>
+      </c>
+      <c r="R4" s="12">
         <v>24.67</v>
       </c>
-      <c r="R4" s="10">
+      <c r="S4" s="12">
         <v>26.59</v>
       </c>
-      <c r="S4" s="10">
+      <c r="T4" s="12">
         <v>4.81</v>
       </c>
-      <c r="T4" s="10">
-        <v>16</v>
-      </c>
-      <c r="U4" s="10">
+      <c r="U4" s="12">
+        <v>16</v>
+      </c>
+      <c r="V4" s="12">
         <v>29.48</v>
       </c>
-      <c r="V4" s="10">
+      <c r="W4" s="12">
         <v>4.96</v>
       </c>
-      <c r="W4" s="10">
-        <v>16</v>
-      </c>
-      <c r="X4" s="10">
+      <c r="X4" s="12">
+        <v>16</v>
+      </c>
+      <c r="Y4" s="12">
         <v>34.44</v>
       </c>
-      <c r="Y4" s="10">
+      <c r="Z4" s="12">
         <v>5.23</v>
       </c>
-      <c r="Z4" s="10">
+      <c r="AA4" s="12">
         <v>17</v>
       </c>
-      <c r="AA4" s="10">
+      <c r="AB4" s="12">
         <v>39.67</v>
       </c>
-      <c r="AB4" s="10">
+      <c r="AC4" s="12">
         <v>5.37</v>
       </c>
-      <c r="AC4" s="10">
+      <c r="AD4" s="12">
         <v>17</v>
       </c>
-      <c r="AD4" s="10">
+      <c r="AE4" s="12">
         <v>45.04</v>
       </c>
-      <c r="AE4" s="10">
+      <c r="AF4" s="12">
         <v>5.84</v>
       </c>
-      <c r="AF4" s="10">
+      <c r="AG4" s="12">
         <v>19</v>
       </c>
-      <c r="AG4" s="10">
+      <c r="AH4" s="12">
         <v>50.88</v>
       </c>
-      <c r="AH4" s="10">
+      <c r="AI4" s="12">
         <v>6.78</v>
       </c>
-      <c r="AI4" s="10">
+      <c r="AJ4" s="12">
         <v>57.66</v>
       </c>
-      <c r="AJ4" s="10">
+      <c r="AK4" s="12">
         <v>26.59</v>
       </c>
-      <c r="AK4" s="10">
+      <c r="AL4" s="12">
         <v>31.07</v>
       </c>
-      <c r="AL4" s="10">
+      <c r="AM4" s="12">
         <v>4.47</v>
       </c>
-      <c r="AM4" s="10">
+      <c r="AN4" s="12">
         <v>4</v>
       </c>
-      <c r="AN4" s="10">
+      <c r="AO4" s="12">
         <v>6</v>
       </c>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="7">
+      <c r="A5" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B5" s="9">
         <v>45444</v>
       </c>
-      <c r="B5" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="C5" t="s" s="9">
-        <v>44</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="C5" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s" s="11">
+        <v>45</v>
+      </c>
+      <c r="E5" s="12">
         <v>23</v>
       </c>
-      <c r="E5" s="10">
+      <c r="F5" s="12">
         <v>6.71</v>
       </c>
-      <c r="F5" s="10">
+      <c r="G5" s="12">
         <v>4.23</v>
       </c>
-      <c r="G5" s="10">
+      <c r="H5" s="12">
         <v>15</v>
       </c>
-      <c r="H5" s="10">
+      <c r="I5" s="12">
         <v>10.94</v>
       </c>
-      <c r="I5" s="10">
+      <c r="J5" s="12">
         <v>4.34</v>
       </c>
-      <c r="J5" s="10">
+      <c r="K5" s="12">
         <v>15</v>
       </c>
-      <c r="K5" s="10">
+      <c r="L5" s="12">
         <v>15.28</v>
       </c>
-      <c r="L5" s="10">
+      <c r="M5" s="12">
         <v>4.52</v>
       </c>
-      <c r="M5" s="10">
-        <v>16</v>
-      </c>
-      <c r="N5" s="10">
+      <c r="N5" s="12">
+        <v>16</v>
+      </c>
+      <c r="O5" s="12">
         <v>19.8</v>
       </c>
-      <c r="O5" s="10">
+      <c r="P5" s="12">
         <v>4.67</v>
       </c>
-      <c r="P5" s="10">
-        <v>16</v>
-      </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="12">
+        <v>16</v>
+      </c>
+      <c r="R5" s="12">
         <v>24.47</v>
       </c>
-      <c r="R5" s="10">
+      <c r="S5" s="12">
         <v>26.37</v>
       </c>
-      <c r="S5" s="10">
+      <c r="T5" s="12">
         <v>4.75</v>
       </c>
-      <c r="T5" s="10">
-        <v>16</v>
-      </c>
-      <c r="U5" s="10">
+      <c r="U5" s="12">
+        <v>16</v>
+      </c>
+      <c r="V5" s="12">
         <v>29.22</v>
       </c>
-      <c r="V5" s="10">
+      <c r="W5" s="12">
         <v>4.94</v>
       </c>
-      <c r="W5" s="10">
-        <v>16</v>
-      </c>
-      <c r="X5" s="10">
+      <c r="X5" s="12">
+        <v>16</v>
+      </c>
+      <c r="Y5" s="12">
         <v>34.16</v>
       </c>
-      <c r="Y5" s="10">
+      <c r="Z5" s="12">
         <v>5.23</v>
       </c>
-      <c r="Z5" s="10">
+      <c r="AA5" s="12">
         <v>17</v>
       </c>
-      <c r="AA5" s="10">
+      <c r="AB5" s="12">
         <v>39.39</v>
       </c>
-      <c r="AB5" s="10">
+      <c r="AC5" s="12">
         <v>5.39</v>
       </c>
-      <c r="AC5" s="10">
+      <c r="AD5" s="12">
         <v>17</v>
       </c>
-      <c r="AD5" s="10">
+      <c r="AE5" s="12">
         <v>44.78</v>
       </c>
-      <c r="AE5" s="10">
+      <c r="AF5" s="12">
         <v>5.56</v>
       </c>
-      <c r="AF5" s="10">
+      <c r="AG5" s="12">
         <v>17</v>
       </c>
-      <c r="AG5" s="10">
+      <c r="AH5" s="12">
         <v>50.34</v>
       </c>
-      <c r="AH5" s="10">
+      <c r="AI5" s="12">
         <v>6.31</v>
       </c>
-      <c r="AI5" s="10">
+      <c r="AJ5" s="12">
         <v>56.65</v>
       </c>
-      <c r="AJ5" s="10">
+      <c r="AK5" s="12">
         <v>26.37</v>
       </c>
-      <c r="AK5" s="10">
+      <c r="AL5" s="12">
         <v>30.28</v>
       </c>
-      <c r="AL5" s="10">
+      <c r="AM5" s="12">
         <v>3.91</v>
       </c>
-      <c r="AM5" s="10">
+      <c r="AN5" s="12">
         <v>1</v>
       </c>
-      <c r="AN5" s="10">
+      <c r="AO5" s="12">
         <v>6</v>
       </c>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="7">
+      <c r="A6" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B6" s="9">
         <v>45452</v>
       </c>
-      <c r="B6" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="C6" t="s" s="9">
-        <v>45</v>
-      </c>
-      <c r="D6" s="10">
+      <c r="C6" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s" s="11">
+        <v>46</v>
+      </c>
+      <c r="E6" s="12">
         <v>23</v>
       </c>
-      <c r="E6" s="10">
+      <c r="F6" s="12">
         <v>6.67</v>
       </c>
-      <c r="F6" s="10">
+      <c r="G6" s="12">
         <v>4.29</v>
       </c>
-      <c r="G6" s="10">
+      <c r="H6" s="12">
         <v>15</v>
       </c>
-      <c r="H6" s="10">
+      <c r="I6" s="12">
         <v>10.96</v>
       </c>
-      <c r="I6" s="10">
+      <c r="J6" s="12">
         <v>4.34</v>
       </c>
-      <c r="J6" s="10">
+      <c r="K6" s="12">
         <v>15</v>
       </c>
-      <c r="K6" s="10">
+      <c r="L6" s="12">
         <v>15.3</v>
       </c>
-      <c r="L6" s="10">
+      <c r="M6" s="12">
         <v>4.55</v>
       </c>
-      <c r="M6" s="10">
-        <v>16</v>
-      </c>
-      <c r="N6" s="10">
+      <c r="N6" s="12">
+        <v>16</v>
+      </c>
+      <c r="O6" s="12">
         <v>19.85</v>
       </c>
-      <c r="O6" s="10">
+      <c r="P6" s="12">
         <v>4.71</v>
       </c>
-      <c r="P6" s="10">
-        <v>16</v>
-      </c>
-      <c r="Q6" s="10">
+      <c r="Q6" s="12">
+        <v>16</v>
+      </c>
+      <c r="R6" s="12">
         <v>24.56</v>
       </c>
-      <c r="R6" s="10">
+      <c r="S6" s="12">
         <v>26.48</v>
       </c>
-      <c r="S6" s="10">
+      <c r="T6" s="12">
         <v>4.8</v>
       </c>
-      <c r="T6" s="10">
-        <v>16</v>
-      </c>
-      <c r="U6" s="10">
+      <c r="U6" s="12">
+        <v>16</v>
+      </c>
+      <c r="V6" s="12">
         <v>29.36</v>
       </c>
-      <c r="V6" s="10">
+      <c r="W6" s="12">
         <v>4.91</v>
       </c>
-      <c r="W6" s="10">
-        <v>16</v>
-      </c>
-      <c r="X6" s="10">
+      <c r="X6" s="12">
+        <v>16</v>
+      </c>
+      <c r="Y6" s="12">
         <v>34.27</v>
       </c>
-      <c r="Y6" s="10">
+      <c r="Z6" s="12">
         <v>5.3</v>
       </c>
-      <c r="Z6" s="10">
+      <c r="AA6" s="12">
         <v>17</v>
       </c>
-      <c r="AA6" s="10">
+      <c r="AB6" s="12">
         <v>39.57</v>
       </c>
-      <c r="AB6" s="10">
+      <c r="AC6" s="12">
         <v>5.29</v>
       </c>
-      <c r="AC6" s="10">
+      <c r="AD6" s="12">
         <v>17</v>
       </c>
-      <c r="AD6" s="10">
+      <c r="AE6" s="12">
         <v>44.86</v>
       </c>
-      <c r="AE6" s="10">
+      <c r="AF6" s="12">
         <v>5.35</v>
       </c>
-      <c r="AF6" s="10">
+      <c r="AG6" s="12">
         <v>17</v>
       </c>
-      <c r="AG6" s="10">
+      <c r="AH6" s="12">
         <v>50.21</v>
       </c>
-      <c r="AH6" s="10">
+      <c r="AI6" s="12">
         <v>6.38</v>
       </c>
-      <c r="AI6" s="10">
+      <c r="AJ6" s="12">
         <v>56.59</v>
       </c>
-      <c r="AJ6" s="10">
+      <c r="AK6" s="12">
         <v>26.48</v>
       </c>
-      <c r="AK6" s="10">
+      <c r="AL6" s="12">
         <v>30.11</v>
       </c>
-      <c r="AL6" s="10">
+      <c r="AM6" s="12">
         <v>3.63</v>
       </c>
-      <c r="AM6" s="10">
+      <c r="AN6" s="12">
         <v>6</v>
       </c>
-      <c r="AN6" s="10">
+      <c r="AO6" s="12">
         <v>5</v>
       </c>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="7">
+      <c r="A7" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B7" s="9">
         <v>45459</v>
       </c>
-      <c r="B7" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s" s="9">
-        <v>46</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C7" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s" s="11">
+        <v>47</v>
+      </c>
+      <c r="E7" s="12">
         <v>23</v>
       </c>
-      <c r="E7" s="10">
+      <c r="F7" s="12">
         <v>6.64</v>
       </c>
-      <c r="F7" s="10">
+      <c r="G7" s="12">
         <v>4.17</v>
       </c>
-      <c r="G7" s="10">
+      <c r="H7" s="12">
         <v>15</v>
       </c>
-      <c r="H7" s="10">
+      <c r="I7" s="12">
         <v>10.81</v>
       </c>
-      <c r="I7" s="10">
+      <c r="J7" s="12">
         <v>4.32</v>
       </c>
-      <c r="J7" s="10">
+      <c r="K7" s="12">
         <v>15</v>
       </c>
-      <c r="K7" s="10">
+      <c r="L7" s="12">
         <v>15.13</v>
       </c>
-      <c r="L7" s="10">
+      <c r="M7" s="12">
         <v>4.55</v>
       </c>
-      <c r="M7" s="10">
-        <v>16</v>
-      </c>
-      <c r="N7" s="10">
+      <c r="N7" s="12">
+        <v>16</v>
+      </c>
+      <c r="O7" s="12">
         <v>19.68</v>
       </c>
-      <c r="O7" s="10">
+      <c r="P7" s="12">
         <v>4.58</v>
       </c>
-      <c r="P7" s="10">
-        <v>16</v>
-      </c>
-      <c r="Q7" s="10">
+      <c r="Q7" s="12">
+        <v>16</v>
+      </c>
+      <c r="R7" s="12">
         <v>24.26</v>
       </c>
-      <c r="R7" s="10">
+      <c r="S7" s="12">
         <v>26.16</v>
       </c>
-      <c r="S7" s="10">
+      <c r="T7" s="12">
         <v>4.76</v>
       </c>
-      <c r="T7" s="10">
-        <v>16</v>
-      </c>
-      <c r="U7" s="10">
+      <c r="U7" s="12">
+        <v>16</v>
+      </c>
+      <c r="V7" s="12">
         <v>29.02</v>
       </c>
-      <c r="V7" s="10">
+      <c r="W7" s="12">
         <v>4.96</v>
       </c>
-      <c r="W7" s="10">
-        <v>16</v>
-      </c>
-      <c r="X7" s="10">
+      <c r="X7" s="12">
+        <v>16</v>
+      </c>
+      <c r="Y7" s="12">
         <v>33.98</v>
       </c>
-      <c r="Y7" s="10">
+      <c r="Z7" s="12">
         <v>5.17</v>
       </c>
-      <c r="Z7" s="10">
+      <c r="AA7" s="12">
         <v>17</v>
       </c>
-      <c r="AA7" s="10">
+      <c r="AB7" s="12">
         <v>39.15</v>
       </c>
-      <c r="AB7" s="10">
+      <c r="AC7" s="12">
         <v>5.31</v>
       </c>
-      <c r="AC7" s="10">
+      <c r="AD7" s="12">
         <v>17</v>
       </c>
-      <c r="AD7" s="10">
+      <c r="AE7" s="12">
         <v>44.46</v>
       </c>
-      <c r="AE7" s="10">
+      <c r="AF7" s="12">
         <v>5.48</v>
       </c>
-      <c r="AF7" s="10">
+      <c r="AG7" s="12">
         <v>17</v>
       </c>
-      <c r="AG7" s="10">
+      <c r="AH7" s="12">
         <v>49.94</v>
       </c>
-      <c r="AH7" s="10">
+      <c r="AI7" s="12">
         <v>6.55</v>
       </c>
-      <c r="AI7" s="10">
+      <c r="AJ7" s="12">
         <v>56.49</v>
       </c>
-      <c r="AJ7" s="10">
+      <c r="AK7" s="12">
         <v>26.16</v>
       </c>
-      <c r="AK7" s="10">
+      <c r="AL7" s="12">
         <v>30.33</v>
       </c>
-      <c r="AL7" s="10">
+      <c r="AM7" s="12">
         <v>4.16</v>
       </c>
-      <c r="AM7" s="10">
+      <c r="AN7" s="12">
         <v>3</v>
       </c>
-      <c r="AN7" s="10">
+      <c r="AO7" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="7">
+      <c r="A8" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B8" s="9">
         <v>45461</v>
       </c>
-      <c r="B8" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="C8" t="s" s="9">
-        <v>47</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="C8" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s" s="11">
+        <v>48</v>
+      </c>
+      <c r="E8" s="12">
         <v>23</v>
       </c>
-      <c r="E8" s="10">
+      <c r="F8" s="12">
         <v>6.61</v>
       </c>
-      <c r="F8" s="10">
+      <c r="G8" s="12">
         <v>4.26</v>
       </c>
-      <c r="G8" s="10">
+      <c r="H8" s="12">
         <v>15</v>
       </c>
-      <c r="H8" s="10">
+      <c r="I8" s="12">
         <v>10.87</v>
       </c>
-      <c r="I8" s="10">
+      <c r="J8" s="12">
         <v>4.29</v>
       </c>
-      <c r="J8" s="10">
+      <c r="K8" s="12">
         <v>15</v>
       </c>
-      <c r="K8" s="10">
+      <c r="L8" s="12">
         <v>15.16</v>
       </c>
-      <c r="L8" s="10">
+      <c r="M8" s="12">
         <v>4.46</v>
       </c>
-      <c r="M8" s="10">
-        <v>16</v>
-      </c>
-      <c r="N8" s="10">
+      <c r="N8" s="12">
+        <v>16</v>
+      </c>
+      <c r="O8" s="12">
         <v>19.62</v>
       </c>
-      <c r="O8" s="10">
+      <c r="P8" s="12">
         <v>4.68</v>
       </c>
-      <c r="P8" s="10">
-        <v>16</v>
-      </c>
-      <c r="Q8" s="10">
+      <c r="Q8" s="12">
+        <v>16</v>
+      </c>
+      <c r="R8" s="12">
         <v>24.3</v>
       </c>
-      <c r="R8" s="10">
+      <c r="S8" s="12">
         <v>26.19</v>
       </c>
-      <c r="S8" s="10">
+      <c r="T8" s="12">
         <v>4.73</v>
       </c>
-      <c r="T8" s="10">
-        <v>16</v>
-      </c>
-      <c r="U8" s="10">
+      <c r="U8" s="12">
+        <v>16</v>
+      </c>
+      <c r="V8" s="12">
         <v>29.03</v>
       </c>
-      <c r="V8" s="10">
+      <c r="W8" s="12">
         <v>4.88</v>
       </c>
-      <c r="W8" s="10">
-        <v>16</v>
-      </c>
-      <c r="X8" s="10">
+      <c r="X8" s="12">
+        <v>16</v>
+      </c>
+      <c r="Y8" s="12">
         <v>33.91</v>
       </c>
-      <c r="Y8" s="10">
+      <c r="Z8" s="12">
         <v>5.12</v>
       </c>
-      <c r="Z8" s="10">
+      <c r="AA8" s="12">
         <v>17</v>
       </c>
-      <c r="AA8" s="10">
+      <c r="AB8" s="12">
         <v>39.03</v>
       </c>
-      <c r="AB8" s="10">
+      <c r="AC8" s="12">
         <v>5.29</v>
       </c>
-      <c r="AC8" s="10">
+      <c r="AD8" s="12">
         <v>17</v>
       </c>
-      <c r="AD8" s="10">
+      <c r="AE8" s="12">
         <v>44.32</v>
       </c>
-      <c r="AE8" s="10">
+      <c r="AF8" s="12">
         <v>5.72</v>
       </c>
-      <c r="AF8" s="10">
+      <c r="AG8" s="12">
         <v>18</v>
       </c>
-      <c r="AG8" s="10">
+      <c r="AH8" s="12">
         <v>50.04</v>
       </c>
-      <c r="AH8" s="10">
+      <c r="AI8" s="12">
         <v>6.56</v>
       </c>
-      <c r="AI8" s="10">
+      <c r="AJ8" s="12">
         <v>56.6</v>
       </c>
-      <c r="AJ8" s="10">
+      <c r="AK8" s="12">
         <v>26.19</v>
       </c>
-      <c r="AK8" s="10">
+      <c r="AL8" s="12">
         <v>30.41</v>
       </c>
-      <c r="AL8" s="10">
+      <c r="AM8" s="12">
         <v>4.22</v>
       </c>
-      <c r="AM8" s="10">
+      <c r="AN8" s="12">
         <v>1</v>
       </c>
-      <c r="AN8" s="10">
+      <c r="AO8" s="12">
         <v>4</v>
       </c>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="7">
+      <c r="A9" s="8">
+        <v>2024</v>
+      </c>
+      <c r="B9" s="9">
         <v>45465</v>
       </c>
-      <c r="B9" t="s" s="8">
-        <v>40</v>
-      </c>
-      <c r="C9" t="s" s="9">
-        <v>48</v>
-      </c>
-      <c r="D9" s="10">
+      <c r="C9" t="s" s="10">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s" s="11">
+        <v>49</v>
+      </c>
+      <c r="E9" s="12">
         <v>23</v>
       </c>
-      <c r="E9" s="10">
+      <c r="F9" s="12">
         <v>6.66</v>
       </c>
-      <c r="F9" s="10">
+      <c r="G9" s="12">
         <v>4.28</v>
       </c>
-      <c r="G9" s="10">
-        <v>16</v>
-      </c>
-      <c r="H9" s="10">
+      <c r="H9" s="12">
+        <v>16</v>
+      </c>
+      <c r="I9" s="12">
         <v>10.94</v>
       </c>
-      <c r="I9" s="10">
+      <c r="J9" s="12">
         <v>4.47</v>
       </c>
-      <c r="J9" s="10">
-        <v>16</v>
-      </c>
-      <c r="K9" s="10">
+      <c r="K9" s="12">
+        <v>16</v>
+      </c>
+      <c r="L9" s="12">
         <v>15.41</v>
       </c>
-      <c r="L9" s="10">
+      <c r="M9" s="12">
         <v>4.48</v>
       </c>
-      <c r="M9" s="10">
-        <v>16</v>
-      </c>
-      <c r="N9" s="10">
+      <c r="N9" s="12">
+        <v>16</v>
+      </c>
+      <c r="O9" s="12">
         <v>19.89</v>
       </c>
-      <c r="O9" s="10">
+      <c r="P9" s="12">
         <v>4.52</v>
       </c>
-      <c r="P9" s="10">
-        <v>16</v>
-      </c>
-      <c r="Q9" s="10">
+      <c r="Q9" s="12">
+        <v>16</v>
+      </c>
+      <c r="R9" s="12">
         <v>24.41</v>
       </c>
-      <c r="R9" s="10">
+      <c r="S9" s="12">
         <v>26.28</v>
       </c>
-      <c r="S9" s="10">
+      <c r="T9" s="12">
         <v>4.67</v>
       </c>
-      <c r="T9" s="10">
-        <v>16</v>
-      </c>
-      <c r="U9" s="10">
+      <c r="U9" s="12">
+        <v>16</v>
+      </c>
+      <c r="V9" s="12">
         <v>29.08</v>
       </c>
-      <c r="V9" s="10">
+      <c r="W9" s="12">
         <v>5</v>
       </c>
-      <c r="W9" s="10">
+      <c r="X9" s="12">
         <v>17</v>
       </c>
-      <c r="X9" s="10">
+      <c r="Y9" s="12">
         <v>34.08</v>
       </c>
-      <c r="Y9" s="10">
+      <c r="Z9" s="12">
         <v>5.19</v>
       </c>
-      <c r="Z9" s="10">
+      <c r="AA9" s="12">
         <v>17</v>
       </c>
-      <c r="AA9" s="10">
+      <c r="AB9" s="12">
         <v>39.27</v>
       </c>
-      <c r="AB9" s="10">
+      <c r="AC9" s="12">
         <v>5.37</v>
       </c>
-      <c r="AC9" s="10">
+      <c r="AD9" s="12">
         <v>18</v>
       </c>
-      <c r="AD9" s="10">
+      <c r="AE9" s="12">
         <v>44.64</v>
       </c>
-      <c r="AE9" s="10">
+      <c r="AF9" s="12">
         <v>5.46</v>
       </c>
-      <c r="AF9" s="10">
+      <c r="AG9" s="12">
         <v>18</v>
       </c>
-      <c r="AG9" s="10">
+      <c r="AH9" s="12">
         <v>50.1</v>
       </c>
-      <c r="AH9" s="10">
+      <c r="AI9" s="12">
         <v>6.41</v>
       </c>
-      <c r="AI9" s="10">
+      <c r="AJ9" s="12">
         <v>56.51</v>
       </c>
-      <c r="AJ9" s="10">
+      <c r="AK9" s="12">
         <v>26.28</v>
       </c>
-      <c r="AK9" s="10">
+      <c r="AL9" s="12">
         <v>30.23</v>
       </c>
-      <c r="AL9" s="10">
+      <c r="AM9" s="12">
         <v>3.95</v>
       </c>
-      <c r="AM9" s="10">
+      <c r="AN9" s="12">
         <v>5</v>
       </c>
-      <c r="AN9" s="10">
+      <c r="AO9" s="12">
         <v>3</v>
       </c>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-      <c r="AB10" s="11"/>
-      <c r="AC10" s="11"/>
-      <c r="AD10" s="11"/>
-      <c r="AE10" s="11"/>
-      <c r="AF10" s="11"/>
-      <c r="AG10" s="11"/>
-      <c r="AH10" s="11"/>
-      <c r="AI10" s="11"/>
-      <c r="AJ10" s="11"/>
-      <c r="AK10" s="11"/>
-      <c r="AL10" s="11"/>
-      <c r="AM10" s="11"/>
-      <c r="AN10" s="11"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
+      <c r="P10" s="13"/>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="13"/>
+      <c r="AM10" s="13"/>
+      <c r="AN10" s="13"/>
+      <c r="AO10" s="13"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-      <c r="AB11" s="11"/>
-      <c r="AC11" s="11"/>
-      <c r="AD11" s="11"/>
-      <c r="AE11" s="11"/>
-      <c r="AF11" s="11"/>
-      <c r="AG11" s="11"/>
-      <c r="AH11" s="11"/>
-      <c r="AI11" s="11"/>
-      <c r="AJ11" s="11"/>
-      <c r="AK11" s="11"/>
-      <c r="AL11" s="11"/>
-      <c r="AM11" s="11"/>
-      <c r="AN11" s="11"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="13"/>
+      <c r="AO11" s="13"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-      <c r="AB12" s="11"/>
-      <c r="AC12" s="11"/>
-      <c r="AD12" s="11"/>
-      <c r="AE12" s="11"/>
-      <c r="AF12" s="11"/>
-      <c r="AG12" s="11"/>
-      <c r="AH12" s="11"/>
-      <c r="AI12" s="11"/>
-      <c r="AJ12" s="11"/>
-      <c r="AK12" s="11"/>
-      <c r="AL12" s="11"/>
-      <c r="AM12" s="11"/>
-      <c r="AN12" s="11"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
+      <c r="P12" s="13"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12" s="13"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="13"/>
+      <c r="AG12" s="13"/>
+      <c r="AH12" s="13"/>
+      <c r="AI12" s="13"/>
+      <c r="AJ12" s="13"/>
+      <c r="AK12" s="13"/>
+      <c r="AL12" s="13"/>
+      <c r="AM12" s="13"/>
+      <c r="AN12" s="13"/>
+      <c r="AO12" s="13"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-      <c r="AB13" s="11"/>
-      <c r="AC13" s="11"/>
-      <c r="AD13" s="11"/>
-      <c r="AE13" s="11"/>
-      <c r="AF13" s="11"/>
-      <c r="AG13" s="11"/>
-      <c r="AH13" s="11"/>
-      <c r="AI13" s="11"/>
-      <c r="AJ13" s="11"/>
-      <c r="AK13" s="11"/>
-      <c r="AL13" s="11"/>
-      <c r="AM13" s="11"/>
-      <c r="AN13" s="11"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="13"/>
+      <c r="S13" s="13"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
+      <c r="AC13" s="13"/>
+      <c r="AD13" s="13"/>
+      <c r="AE13" s="13"/>
+      <c r="AF13" s="13"/>
+      <c r="AG13" s="13"/>
+      <c r="AH13" s="13"/>
+      <c r="AI13" s="13"/>
+      <c r="AJ13" s="13"/>
+      <c r="AK13" s="13"/>
+      <c r="AL13" s="13"/>
+      <c r="AM13" s="13"/>
+      <c r="AN13" s="13"/>
+      <c r="AO13" s="13"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="12"/>
-      <c r="B14" s="13"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-      <c r="AB14" s="11"/>
-      <c r="AC14" s="11"/>
-      <c r="AD14" s="11"/>
-      <c r="AE14" s="11"/>
-      <c r="AF14" s="11"/>
-      <c r="AG14" s="11"/>
-      <c r="AH14" s="11"/>
-      <c r="AI14" s="11"/>
-      <c r="AJ14" s="11"/>
-      <c r="AK14" s="11"/>
-      <c r="AL14" s="11"/>
-      <c r="AM14" s="11"/>
-      <c r="AN14" s="11"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
+      <c r="P14" s="13"/>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
+      <c r="S14" s="13"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="13"/>
+      <c r="AE14" s="13"/>
+      <c r="AF14" s="13"/>
+      <c r="AG14" s="13"/>
+      <c r="AH14" s="13"/>
+      <c r="AI14" s="13"/>
+      <c r="AJ14" s="13"/>
+      <c r="AK14" s="13"/>
+      <c r="AL14" s="13"/>
+      <c r="AM14" s="13"/>
+      <c r="AN14" s="13"/>
+      <c r="AO14" s="13"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
-      <c r="AB15" s="11"/>
-      <c r="AC15" s="11"/>
-      <c r="AD15" s="11"/>
-      <c r="AE15" s="11"/>
-      <c r="AF15" s="11"/>
-      <c r="AG15" s="11"/>
-      <c r="AH15" s="11"/>
-      <c r="AI15" s="11"/>
-      <c r="AJ15" s="11"/>
-      <c r="AK15" s="11"/>
-      <c r="AL15" s="11"/>
-      <c r="AM15" s="11"/>
-      <c r="AN15" s="11"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
+      <c r="P15" s="13"/>
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15" s="13"/>
+      <c r="T15" s="13"/>
+      <c r="U15" s="13"/>
+      <c r="V15" s="13"/>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="13"/>
+      <c r="AD15" s="13"/>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="13"/>
+      <c r="AG15" s="13"/>
+      <c r="AH15" s="13"/>
+      <c r="AI15" s="13"/>
+      <c r="AJ15" s="13"/>
+      <c r="AK15" s="13"/>
+      <c r="AL15" s="13"/>
+      <c r="AM15" s="13"/>
+      <c r="AN15" s="13"/>
+      <c r="AO15" s="13"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="12"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
-      <c r="AI16" s="11"/>
-      <c r="AJ16" s="11"/>
-      <c r="AK16" s="11"/>
-      <c r="AL16" s="11"/>
-      <c r="AM16" s="11"/>
-      <c r="AN16" s="11"/>
+      <c r="A16" s="14"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="13"/>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="13"/>
+      <c r="AE16" s="13"/>
+      <c r="AF16" s="13"/>
+      <c r="AG16" s="13"/>
+      <c r="AH16" s="13"/>
+      <c r="AI16" s="13"/>
+      <c r="AJ16" s="13"/>
+      <c r="AK16" s="13"/>
+      <c r="AL16" s="13"/>
+      <c r="AM16" s="13"/>
+      <c r="AN16" s="13"/>
+      <c r="AO16" s="13"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
-      <c r="AB17" s="11"/>
-      <c r="AC17" s="11"/>
-      <c r="AD17" s="11"/>
-      <c r="AE17" s="11"/>
-      <c r="AF17" s="11"/>
-      <c r="AG17" s="11"/>
-      <c r="AH17" s="11"/>
-      <c r="AI17" s="11"/>
-      <c r="AJ17" s="11"/>
-      <c r="AK17" s="11"/>
-      <c r="AL17" s="11"/>
-      <c r="AM17" s="11"/>
-      <c r="AN17" s="11"/>
+      <c r="A17" s="14"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="13"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="13"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="13"/>
+      <c r="AH17" s="13"/>
+      <c r="AI17" s="13"/>
+      <c r="AJ17" s="13"/>
+      <c r="AK17" s="13"/>
+      <c r="AL17" s="13"/>
+      <c r="AM17" s="13"/>
+      <c r="AN17" s="13"/>
+      <c r="AO17" s="13"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="12"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
-      <c r="AB18" s="11"/>
-      <c r="AC18" s="11"/>
-      <c r="AD18" s="11"/>
-      <c r="AE18" s="11"/>
-      <c r="AF18" s="11"/>
-      <c r="AG18" s="11"/>
-      <c r="AH18" s="11"/>
-      <c r="AI18" s="11"/>
-      <c r="AJ18" s="11"/>
-      <c r="AK18" s="11"/>
-      <c r="AL18" s="11"/>
-      <c r="AM18" s="11"/>
-      <c r="AN18" s="11"/>
+      <c r="A18" s="14"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+      <c r="AB18" s="13"/>
+      <c r="AC18" s="13"/>
+      <c r="AD18" s="13"/>
+      <c r="AE18" s="13"/>
+      <c r="AF18" s="13"/>
+      <c r="AG18" s="13"/>
+      <c r="AH18" s="13"/>
+      <c r="AI18" s="13"/>
+      <c r="AJ18" s="13"/>
+      <c r="AK18" s="13"/>
+      <c r="AL18" s="13"/>
+      <c r="AM18" s="13"/>
+      <c r="AN18" s="13"/>
+      <c r="AO18" s="13"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="12"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
-      <c r="AB19" s="11"/>
-      <c r="AC19" s="11"/>
-      <c r="AD19" s="11"/>
-      <c r="AE19" s="11"/>
-      <c r="AF19" s="11"/>
-      <c r="AG19" s="11"/>
-      <c r="AH19" s="11"/>
-      <c r="AI19" s="11"/>
-      <c r="AJ19" s="11"/>
-      <c r="AK19" s="11"/>
-      <c r="AL19" s="11"/>
-      <c r="AM19" s="11"/>
-      <c r="AN19" s="11"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="13"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
+      <c r="AC19" s="13"/>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
+      <c r="AF19" s="13"/>
+      <c r="AG19" s="13"/>
+      <c r="AH19" s="13"/>
+      <c r="AI19" s="13"/>
+      <c r="AJ19" s="13"/>
+      <c r="AK19" s="13"/>
+      <c r="AL19" s="13"/>
+      <c r="AM19" s="13"/>
+      <c r="AN19" s="13"/>
+      <c r="AO19" s="13"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="11"/>
-      <c r="AB20" s="11"/>
-      <c r="AC20" s="11"/>
-      <c r="AD20" s="11"/>
-      <c r="AE20" s="11"/>
-      <c r="AF20" s="11"/>
-      <c r="AG20" s="11"/>
-      <c r="AH20" s="11"/>
-      <c r="AI20" s="11"/>
-      <c r="AJ20" s="11"/>
-      <c r="AK20" s="11"/>
-      <c r="AL20" s="11"/>
-      <c r="AM20" s="11"/>
-      <c r="AN20" s="11"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="13"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13"/>
+      <c r="AC20" s="13"/>
+      <c r="AD20" s="13"/>
+      <c r="AE20" s="13"/>
+      <c r="AF20" s="13"/>
+      <c r="AG20" s="13"/>
+      <c r="AH20" s="13"/>
+      <c r="AI20" s="13"/>
+      <c r="AJ20" s="13"/>
+      <c r="AK20" s="13"/>
+      <c r="AL20" s="13"/>
+      <c r="AM20" s="13"/>
+      <c r="AN20" s="13"/>
+      <c r="AO20" s="13"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="12"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-      <c r="AA21" s="11"/>
-      <c r="AB21" s="11"/>
-      <c r="AC21" s="11"/>
-      <c r="AD21" s="11"/>
-      <c r="AE21" s="11"/>
-      <c r="AF21" s="11"/>
-      <c r="AG21" s="11"/>
-      <c r="AH21" s="11"/>
-      <c r="AI21" s="11"/>
-      <c r="AJ21" s="11"/>
-      <c r="AK21" s="11"/>
-      <c r="AL21" s="11"/>
-      <c r="AM21" s="11"/>
-      <c r="AN21" s="11"/>
+      <c r="A21" s="14"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="13"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13"/>
+      <c r="AD21" s="13"/>
+      <c r="AE21" s="13"/>
+      <c r="AF21" s="13"/>
+      <c r="AG21" s="13"/>
+      <c r="AH21" s="13"/>
+      <c r="AI21" s="13"/>
+      <c r="AJ21" s="13"/>
+      <c r="AK21" s="13"/>
+      <c r="AL21" s="13"/>
+      <c r="AM21" s="13"/>
+      <c r="AN21" s="13"/>
+      <c r="AO21" s="13"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
-      <c r="AB22" s="11"/>
-      <c r="AC22" s="11"/>
-      <c r="AD22" s="11"/>
-      <c r="AE22" s="11"/>
-      <c r="AF22" s="11"/>
-      <c r="AG22" s="11"/>
-      <c r="AH22" s="11"/>
-      <c r="AI22" s="11"/>
-      <c r="AJ22" s="11"/>
-      <c r="AK22" s="11"/>
-      <c r="AL22" s="11"/>
-      <c r="AM22" s="11"/>
-      <c r="AN22" s="11"/>
+      <c r="A22" s="14"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="13"/>
+      <c r="AD22" s="13"/>
+      <c r="AE22" s="13"/>
+      <c r="AF22" s="13"/>
+      <c r="AG22" s="13"/>
+      <c r="AH22" s="13"/>
+      <c r="AI22" s="13"/>
+      <c r="AJ22" s="13"/>
+      <c r="AK22" s="13"/>
+      <c r="AL22" s="13"/>
+      <c r="AM22" s="13"/>
+      <c r="AN22" s="13"/>
+      <c r="AO22" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>